<commit_message>
haven't committed in forever sorry
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,504 +426,504 @@
     </row>
     <row r="3" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C3" s="5">
-        <v>5000</v>
+        <v>50000</v>
       </c>
       <c r="D3" s="5">
-        <f>5039</f>
-        <v>5039</v>
+        <f>50039</f>
+        <v>50039</v>
       </c>
       <c r="E3" s="5">
-        <v>5078</v>
+        <v>50078</v>
       </c>
     </row>
     <row r="4" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="5">
         <f>C3+1</f>
-        <v>5001</v>
+        <v>50001</v>
       </c>
       <c r="D4" s="5">
         <f>D3+1</f>
-        <v>5040</v>
+        <v>50040</v>
       </c>
       <c r="E4" s="5">
         <f>E3+1</f>
-        <v>5079</v>
+        <v>50079</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <f t="shared" ref="C5:C38" si="0">C4+1</f>
-        <v>5002</v>
+        <v>50002</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" ref="D5:D38" si="1">D4+1</f>
-        <v>5041</v>
+        <v>50041</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" ref="E5:E38" si="2">E4+1</f>
-        <v>5080</v>
+        <v>50080</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>5003</v>
+        <v>50003</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="1"/>
-        <v>5042</v>
+        <v>50042</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="2"/>
-        <v>5081</v>
+        <v>50081</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="5">
         <f t="shared" si="0"/>
-        <v>5004</v>
+        <v>50004</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="1"/>
-        <v>5043</v>
+        <v>50043</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="2"/>
-        <v>5082</v>
+        <v>50082</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>5005</v>
+        <v>50005</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="1"/>
-        <v>5044</v>
+        <v>50044</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="2"/>
-        <v>5083</v>
+        <v>50083</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>5006</v>
+        <v>50006</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="1"/>
-        <v>5045</v>
+        <v>50045</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="2"/>
-        <v>5084</v>
+        <v>50084</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10" s="5">
         <f t="shared" si="0"/>
-        <v>5007</v>
+        <v>50007</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="1"/>
-        <v>5046</v>
+        <v>50046</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="2"/>
-        <v>5085</v>
+        <v>50085</v>
       </c>
     </row>
     <row r="11" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>5008</v>
+        <v>50008</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="1"/>
-        <v>5047</v>
+        <v>50047</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="2"/>
-        <v>5086</v>
+        <v>50086</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>5009</v>
+        <v>50009</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="1"/>
-        <v>5048</v>
+        <v>50048</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" si="2"/>
-        <v>5087</v>
+        <v>50087</v>
       </c>
     </row>
     <row r="13" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>5010</v>
+        <v>50010</v>
       </c>
       <c r="D13" s="5">
         <f t="shared" si="1"/>
-        <v>5049</v>
+        <v>50049</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="2"/>
-        <v>5088</v>
+        <v>50088</v>
       </c>
     </row>
     <row r="14" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>5011</v>
+        <v>50011</v>
       </c>
       <c r="D14" s="5">
         <f t="shared" si="1"/>
-        <v>5050</v>
+        <v>50050</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="2"/>
-        <v>5089</v>
+        <v>50089</v>
       </c>
     </row>
     <row r="15" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>5012</v>
+        <v>50012</v>
       </c>
       <c r="D15" s="5">
         <f t="shared" si="1"/>
-        <v>5051</v>
+        <v>50051</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="2"/>
-        <v>5090</v>
+        <v>50090</v>
       </c>
     </row>
     <row r="16" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>5013</v>
+        <v>50013</v>
       </c>
       <c r="D16" s="5">
         <f t="shared" si="1"/>
-        <v>5052</v>
+        <v>50052</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="2"/>
-        <v>5091</v>
+        <v>50091</v>
       </c>
     </row>
     <row r="17" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>5014</v>
+        <v>50014</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="1"/>
-        <v>5053</v>
+        <v>50053</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" si="2"/>
-        <v>5092</v>
+        <v>50092</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>5015</v>
+        <v>50015</v>
       </c>
       <c r="D18" s="5">
         <f t="shared" si="1"/>
-        <v>5054</v>
+        <v>50054</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="2"/>
-        <v>5093</v>
+        <v>50093</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
-        <v>5016</v>
+        <v>50016</v>
       </c>
       <c r="D19" s="5">
         <f t="shared" si="1"/>
-        <v>5055</v>
+        <v>50055</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="2"/>
-        <v>5094</v>
+        <v>50094</v>
       </c>
     </row>
     <row r="20" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
-        <v>5017</v>
+        <v>50017</v>
       </c>
       <c r="D20" s="5">
         <f t="shared" si="1"/>
-        <v>5056</v>
+        <v>50056</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="2"/>
-        <v>5095</v>
+        <v>50095</v>
       </c>
     </row>
     <row r="21" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
-        <v>5018</v>
+        <v>50018</v>
       </c>
       <c r="D21" s="5">
         <f t="shared" si="1"/>
-        <v>5057</v>
+        <v>50057</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" si="2"/>
-        <v>5096</v>
+        <v>50096</v>
       </c>
     </row>
     <row r="22" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
-        <v>5019</v>
+        <v>50019</v>
       </c>
       <c r="D22" s="5">
         <f t="shared" si="1"/>
-        <v>5058</v>
+        <v>50058</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" si="2"/>
-        <v>5097</v>
+        <v>50097</v>
       </c>
     </row>
     <row r="23" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
-        <v>5020</v>
+        <v>50020</v>
       </c>
       <c r="D23" s="5">
         <f t="shared" si="1"/>
-        <v>5059</v>
+        <v>50059</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" si="2"/>
-        <v>5098</v>
+        <v>50098</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
-        <v>5021</v>
+        <v>50021</v>
       </c>
       <c r="D24" s="5">
         <f t="shared" si="1"/>
-        <v>5060</v>
+        <v>50060</v>
       </c>
       <c r="E24" s="5">
         <f t="shared" si="2"/>
-        <v>5099</v>
+        <v>50099</v>
       </c>
     </row>
     <row r="25" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
-        <v>5022</v>
-      </c>
-      <c r="D25" s="4">
-        <f t="shared" si="1"/>
-        <v>5061</v>
-      </c>
-      <c r="E25" s="2">
-        <f t="shared" si="2"/>
-        <v>5100</v>
+        <v>50022</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="1"/>
+        <v>50061</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="2"/>
+        <v>50100</v>
       </c>
     </row>
     <row r="26" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
-        <v>5023</v>
-      </c>
-      <c r="D26" s="4">
-        <f t="shared" si="1"/>
-        <v>5062</v>
+        <v>50023</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="1"/>
+        <v>50062</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="2"/>
-        <v>5101</v>
+        <v>50101</v>
       </c>
     </row>
     <row r="27" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
-        <v>5024</v>
+        <v>50024</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="1"/>
-        <v>5063</v>
+        <v>50063</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="2"/>
-        <v>5102</v>
+        <v>50102</v>
       </c>
     </row>
     <row r="28" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
-        <v>5025</v>
+        <v>50025</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="1"/>
-        <v>5064</v>
+        <v>50064</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="2"/>
-        <v>5103</v>
+        <v>50103</v>
       </c>
     </row>
     <row r="29" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
-        <v>5026</v>
+        <v>50026</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="1"/>
-        <v>5065</v>
+        <v>50065</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="2"/>
-        <v>5104</v>
+        <v>50104</v>
       </c>
     </row>
     <row r="30" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
-        <v>5027</v>
+        <v>50027</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="1"/>
-        <v>5066</v>
+        <v>50066</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="2"/>
-        <v>5105</v>
+        <v>50105</v>
       </c>
     </row>
     <row r="31" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
-        <v>5028</v>
+        <v>50028</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="1"/>
-        <v>5067</v>
+        <v>50067</v>
       </c>
       <c r="E31" s="5">
         <f t="shared" si="2"/>
-        <v>5106</v>
+        <v>50106</v>
       </c>
     </row>
     <row r="32" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
-        <v>5029</v>
+        <v>50029</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="1"/>
-        <v>5068</v>
+        <v>50068</v>
       </c>
       <c r="E32" s="5">
         <f t="shared" si="2"/>
-        <v>5107</v>
+        <v>50107</v>
       </c>
     </row>
     <row r="33" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
-        <v>5030</v>
+        <v>50030</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="1"/>
-        <v>5069</v>
+        <v>50069</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="2"/>
-        <v>5108</v>
+        <v>50108</v>
       </c>
     </row>
     <row r="34" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
-        <v>5031</v>
+        <v>50031</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="1"/>
-        <v>5070</v>
+        <v>50070</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="2"/>
-        <v>5109</v>
+        <v>50109</v>
       </c>
     </row>
     <row r="35" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
-        <v>5032</v>
+        <v>50032</v>
       </c>
       <c r="D35" s="4">
         <f t="shared" si="1"/>
-        <v>5071</v>
+        <v>50071</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="2"/>
-        <v>5110</v>
+        <v>50110</v>
       </c>
     </row>
     <row r="36" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
-        <v>5033</v>
+        <v>50033</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="1"/>
-        <v>5072</v>
+        <v>50072</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="2"/>
-        <v>5111</v>
+        <v>50111</v>
       </c>
     </row>
     <row r="37" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
-        <v>5034</v>
+        <v>50034</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="1"/>
-        <v>5073</v>
+        <v>50073</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="2"/>
-        <v>5112</v>
+        <v>50112</v>
       </c>
     </row>
     <row r="38" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C38" s="2">
-        <f t="shared" si="0"/>
-        <v>5035</v>
+      <c r="C38" s="5">
+        <f t="shared" si="0"/>
+        <v>50035</v>
       </c>
       <c r="D38" s="4">
         <f t="shared" si="1"/>
-        <v>5074</v>
+        <v>50074</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="2"/>
-        <v>5113</v>
+        <v>50113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>